<commit_message>
Added script to create diagrams from source code using pyReverse and GraphViz. Instructions for installing pyReverse (Part of the Pylint package) and GraphViz are in the readme.txt in docs\Class_Diagram_Tool
</commit_message>
<xml_diff>
--- a/docs/Document Table.xlsx
+++ b/docs/Document Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bfreeman\Documents\ModelCatalog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgould\Documents\ModelCatalog\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{209DD14B-E089-405B-9456-DBBDFD0538BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F502254F-D2FF-436F-80A1-A32C60EE4B6F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{7BD1DB24-80EA-454E-A892-E0C055D34D67}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Capabilities</t>
   </si>
@@ -36,21 +36,12 @@
     <t>Planned</t>
   </si>
   <si>
-    <t>Record Project Number</t>
-  </si>
-  <si>
     <t>Allows input for Project types of Combined, Sanitary, Storm and User Defined</t>
   </si>
   <si>
     <t>Accepts Model Purpose of Calibration, Characterization, Alternative, Recommended Plan</t>
   </si>
   <si>
-    <t>Prompts for and Accepts Calibration File path for use with Calibration Model</t>
-  </si>
-  <si>
-    <t>Pull Model from user defined Directory path</t>
-  </si>
-  <si>
     <t>Allows Optional Model Alterations of Boundary Conditions, Regression Equations and Roughness</t>
   </si>
   <si>
@@ -60,25 +51,33 @@
     <t>Prompts for and Accepts, Model Alterations File when Model Alterations are selected</t>
   </si>
   <si>
-    <t>Calibrates Model using parameters pin provided Excel file path</t>
-  </si>
-  <si>
     <t>Prompts for Model Status of Working or Final</t>
   </si>
   <si>
-    <t>Model is Altered using provided Alterations file</t>
-  </si>
-  <si>
     <t>Accepts Project Phases of: Planning, Pre-Design, 30, 60, and 90 percent</t>
   </si>
   <si>
     <t>Working Models are registered in Model Catalog</t>
   </si>
   <si>
-    <t>Final Models are registered in RRAD</t>
-  </si>
-  <si>
-    <t>RRAD Subsets Stroms</t>
+    <t>Stores user defined Model Directory Path</t>
+  </si>
+  <si>
+    <t>Records Project Number/Model Work Order Number</t>
+  </si>
+  <si>
+    <t>Prompts for and Stores Calibration File path if  Model Purpose: Calibration is selected</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Option available in GUI
+DB Table Exists
+Code still required</t>
+  </si>
+  <si>
+    <t>Final Models are registered in Model Catalog and capacity results are copied to RRAD</t>
   </si>
 </sst>
 </file>
@@ -239,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -285,6 +284,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F27845A-8D4B-40FE-815D-F493AE3920E8}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,9 +619,10 @@
     <col min="1" max="1" width="50.140625" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -623,138 +632,144 @@
       <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="17"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="17"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="18"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -809,45 +824,25 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>